<commit_message>
se avanzo y se termino el consolidao de precios
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gonzalo PL\Desktop\Automatizaciones\Automatizacione-EMP1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6650DE4-FEEF-4FC5-9963-33A8337F43A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{319F66C7-DA12-4969-B2D2-F8EB9C314AC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5220" yWindow="2325" windowWidth="22710" windowHeight="12570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,12 +25,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>RUTA DE ARCHIVO DE EXCEL</t>
   </si>
   <si>
     <t>C:\Users\Gonzalo PL\Desktop\Automatizaciones\Automatizacione-EMP1</t>
+  </si>
+  <si>
+    <t>rutaCRM</t>
+  </si>
+  <si>
+    <t>LISTA PRECIOS</t>
+  </si>
+  <si>
+    <t>LISTA PRECIOS LG</t>
+  </si>
+  <si>
+    <t>C:\Users\Gonzalo PL\Desktop\Automatizaciones\Automatizacione-EMP1\Codigos Costos\LISTA DE PRECIOS LG - VENTAS COSTOS 30.10.25- OCTUBRE 2025.xlsx</t>
+  </si>
+  <si>
+    <t>C:\Users\Gonzalo PL\Desktop\Automatizaciones\Automatizacione-EMP1\Codigos Costos\LISTA DE PRECIOS - VENTAS COSTOS 20.10.25- OCTUBRE 2025-4.xlsx</t>
   </si>
 </sst>
 </file>
@@ -46,7 +61,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -59,8 +74,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -68,13 +95,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -355,25 +400,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:B3"/>
+  <dimension ref="A2:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="66.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="142.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>